<commit_message>
Added "DriverLicenseCardIdentification" to NIEM Subset
</commit_message>
<xml_diff>
--- a/shared/ojb-resources-common/src/main/resources/ssp/Court_Case_Search_Request/artifacts/service_model/information_model/IEPD/documentation/Mapping.xlsx
+++ b/shared/ojb-resources-common/src/main/resources/ssp/Court_Case_Search_Request/artifacts/service_model/information_model/IEPD/documentation/Mapping.xlsx
@@ -138,12 +138,6 @@
     <t>ccs-req-doc:CourtCaseSearchRequest/nc:Person/nc:PersonSSNIdentification/nc:IdentificationID</t>
   </si>
   <si>
-    <t>ccs-req-doc:CourtCaseSearchRequest/nc:Person/j:PersonAugmentation/j:DriverLicense/j:DriverLicenseCardIdentification/nc:IdentificationID</t>
-  </si>
-  <si>
-    <t>ccs-req-doc:CourtCaseSearchRequest/nc:Person/j:PersonAugmentation/j:DriverLicense/j:DriverLicenseCardIdentification/nc:IdentificationSourceText</t>
-  </si>
-  <si>
     <t>ccs-req-doc:CourtCaseSearchRequest/nc:Person/j:PersonAugmentation/j:PersonStateFingerprintIdentification/nc:IdentificationID</t>
   </si>
   <si>
@@ -220,6 +214,12 @@
   </si>
   <si>
     <t>Person Record ID</t>
+  </si>
+  <si>
+    <t>ccs-req-doc:CourtCaseSearchRequest/nc:Person/j:PersonAugmentation/j:DriverLicense/j:DriverLicenseIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>ccs-req-doc:CourtCaseSearchRequest/nc:Person/j:PersonAugmentation/j:DriverLicense/j:DriverLicenseIdentification/nc:IdentificationSourceText</t>
   </si>
 </sst>
 </file>
@@ -2225,8 +2225,8 @@
   <dimension ref="A1:C351"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B23" sqref="B23"/>
+      <pane ySplit="2" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2267,7 +2267,7 @@
         <v>9</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -2275,7 +2275,7 @@
         <v>10</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -2283,7 +2283,7 @@
         <v>5</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -2291,15 +2291,15 @@
         <v>11</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="30">
       <c r="B8" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -2378,7 +2378,7 @@
         <v>20</v>
       </c>
       <c r="C18" s="13" t="s">
-        <v>39</v>
+        <v>65</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="45">
@@ -2386,7 +2386,7 @@
         <v>21</v>
       </c>
       <c r="C19" s="13" t="s">
-        <v>40</v>
+        <v>66</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="45">
@@ -2394,15 +2394,15 @@
         <v>22</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="B21" s="10" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="30">
@@ -2410,7 +2410,7 @@
         <v>23</v>
       </c>
       <c r="C22" s="12" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -2418,7 +2418,7 @@
         <v>0</v>
       </c>
       <c r="C23" s="12" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -2426,7 +2426,7 @@
         <v>24</v>
       </c>
       <c r="C24" s="12" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="25" spans="1:3">
@@ -2434,7 +2434,7 @@
         <v>25</v>
       </c>
       <c r="C25" s="11" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="26" spans="1:3">
@@ -2442,7 +2442,7 @@
         <v>26</v>
       </c>
       <c r="C26" s="13" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="45">
@@ -2450,7 +2450,7 @@
         <v>27</v>
       </c>
       <c r="C27" s="13" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="45">
@@ -2458,7 +2458,7 @@
         <v>28</v>
       </c>
       <c r="C28" s="13" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="45">
@@ -2466,7 +2466,7 @@
         <v>29</v>
       </c>
       <c r="C29" s="13" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="45">
@@ -2474,7 +2474,7 @@
         <v>30</v>
       </c>
       <c r="C30" s="13" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="31" spans="1:3">
@@ -2491,34 +2491,34 @@
     </row>
     <row r="33" spans="1:3">
       <c r="B33" s="19" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C33" s="8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="34" spans="1:3">
       <c r="B34" s="19" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C34" s="8" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="35" spans="1:3">
       <c r="B35" s="14" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C35" s="8" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="36" spans="1:3">
       <c r="B36" s="19" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C36" s="9" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="37" spans="1:3">

</xml_diff>